<commit_message>
I've refactored the code to simplify exception handling and comments. Here's a breakdown of the changes:
- I modified `trading_env.py` to throw an exception if the data is missing, instructing you to use `pull_data.py` to download the data.
- I reduced unnecessary try-catch blocks to simplify the codebase.
- I removed unnecessary comments and examples from comments.
</commit_message>
<xml_diff>
--- a/reports/policy_comparison_report.xlsx
+++ b/reports/policy_comparison_report.xlsx
@@ -531,19 +531,19 @@
         <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>10537.09555155619</v>
+        <v>10537.09779531127</v>
       </c>
       <c r="C3" s="2">
         <v>10500</v>
       </c>
       <c r="D3" s="2">
-        <v>37.09555155619091</v>
+        <v>37.09779531126696</v>
       </c>
       <c r="E3" s="3">
-        <v>5.875167890148028</v>
+        <v>5.87518363538967</v>
       </c>
       <c r="F3" s="4">
-        <v>-0.02422770871202247</v>
+        <v>-0.02422770655517628</v>
       </c>
       <c r="G3" s="1">
         <v>10</v>
@@ -554,16 +554,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="2">
-        <v>10433.34136962891</v>
+        <v>10433.3415222168</v>
       </c>
       <c r="C4" s="2">
         <v>10500</v>
       </c>
       <c r="D4" s="2">
-        <v>-66.65863037109375</v>
+        <v>-66.65847778320312</v>
       </c>
       <c r="E4" s="3">
-        <v>53.67864795963109</v>
+        <v>53.67874470157258</v>
       </c>
       <c r="F4" s="4">
         <v>0</v>
@@ -617,7 +617,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>85.90139770507812</v>
+        <v>85.90139007568359</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -657,7 +657,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>86.25180816650391</v>
+        <v>86.25180053710938</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -677,7 +677,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>88.83446502685547</v>
+        <v>88.83444976806641</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -697,7 +697,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>89.82654571533203</v>
+        <v>89.82655334472656</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -717,7 +717,7 @@
         <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>87.81401824951172</v>
+        <v>87.81401062011719</v>
       </c>
       <c r="C7" s="3">
         <v>0</v>
@@ -737,7 +737,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>86.81147766113281</v>
+        <v>86.81148529052734</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -757,7 +757,7 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>87.20166015625</v>
+        <v>87.20166778564453</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
@@ -777,7 +777,7 @@
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>86.49485778808594</v>
+        <v>86.49486541748047</v>
       </c>
       <c r="C10" s="3">
         <v>0</v>
@@ -797,7 +797,7 @@
         <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C11" s="3">
         <v>0</v>
@@ -817,7 +817,7 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C12" s="3">
         <v>0</v>
@@ -874,7 +874,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>85.90139770507812</v>
+        <v>85.90139007568359</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -886,7 +886,7 @@
         <v>10000</v>
       </c>
       <c r="F2" s="3">
-        <v>110.591911315918</v>
+        <v>110.591926574707</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -897,16 +897,16 @@
         <v>86.53163909912109</v>
       </c>
       <c r="C3" s="3">
-        <v>110.591911315918</v>
+        <v>110.591926574707</v>
       </c>
       <c r="D3" s="2">
-        <v>550.0002430866007</v>
+        <v>549.9997760847327</v>
       </c>
       <c r="E3" s="2">
-        <v>10119.69960035762</v>
+        <v>10119.70045372378</v>
       </c>
       <c r="F3" s="3">
-        <v>6.038256645202637</v>
+        <v>6.038250923156738</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -914,19 +914,19 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>86.25180816650391</v>
+        <v>86.25180053710938</v>
       </c>
       <c r="C4" s="3">
-        <v>116.6301651000977</v>
+        <v>116.6301803588867</v>
       </c>
       <c r="D4" s="2">
-        <v>77.49999827605643</v>
+        <v>77.50002641219908</v>
       </c>
       <c r="E4" s="2">
-        <v>10137.06262491736</v>
+        <v>10137.06307933399</v>
       </c>
       <c r="F4" s="3">
-        <v>0.8536052703857422</v>
+        <v>0.8536056280136108</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -934,19 +934,19 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>88.83446502685547</v>
+        <v>88.83444976806641</v>
       </c>
       <c r="C5" s="3">
-        <v>117.483772277832</v>
+        <v>117.4837875366211</v>
       </c>
       <c r="D5" s="2">
-        <v>53.8750002448287</v>
+        <v>53.87500404741513</v>
       </c>
       <c r="E5" s="2">
-        <v>10490.48305988295</v>
+        <v>10490.48262653157</v>
       </c>
       <c r="F5" s="3">
-        <v>0.5761417746543884</v>
+        <v>0.5761419534683228</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -954,19 +954,19 @@
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>89.82654571533203</v>
+        <v>89.82655334472656</v>
       </c>
       <c r="C6" s="3">
-        <v>118.0599136352539</v>
+        <v>118.059928894043</v>
       </c>
       <c r="D6" s="2">
-        <v>52.69375391378298</v>
+        <v>52.69375062275776</v>
       </c>
       <c r="E6" s="2">
-        <v>10657.60798321907</v>
+        <v>10657.61025129813</v>
       </c>
       <c r="F6" s="3">
-        <v>0.5572858452796936</v>
+        <v>0.5572857856750488</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -974,16 +974,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>87.81401824951172</v>
+        <v>87.81401062011719</v>
       </c>
       <c r="C7" s="3">
-        <v>118.6172027587891</v>
+        <v>118.6172180175781</v>
       </c>
       <c r="D7" s="2">
-        <v>52.63469145625913</v>
+        <v>52.63468926756013</v>
       </c>
       <c r="E7" s="2">
-        <v>10468.88789922259</v>
+        <v>10468.88833199192</v>
       </c>
       <c r="F7" s="3">
         <v>0.5694188475608826</v>
@@ -994,16 +994,16 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>86.81147766113281</v>
+        <v>86.81148529052734</v>
       </c>
       <c r="C8" s="3">
-        <v>119.1866226196289</v>
+        <v>119.186637878418</v>
       </c>
       <c r="D8" s="2">
-        <v>52.63173438493186</v>
+        <v>52.6317365405539</v>
       </c>
       <c r="E8" s="2">
-        <v>10399.39856143471</v>
+        <v>10399.40079755024</v>
       </c>
       <c r="F8" s="3">
         <v>0.5759623646736145</v>
@@ -1014,19 +1014,19 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>87.20166015625</v>
+        <v>87.20166778564453</v>
       </c>
       <c r="C9" s="3">
-        <v>119.7625885009766</v>
+        <v>119.7626037597656</v>
       </c>
       <c r="D9" s="2">
-        <v>52.63159043041514</v>
+        <v>52.63158819179307</v>
       </c>
       <c r="E9" s="2">
-        <v>10496.12813232539</v>
+        <v>10496.13037439466</v>
       </c>
       <c r="F9" s="3">
-        <v>0.5733836889266968</v>
+        <v>0.573383629322052</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1034,19 +1034,19 @@
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>86.49485778808594</v>
+        <v>86.49486541748047</v>
       </c>
       <c r="C10" s="3">
-        <v>120.3359756469727</v>
+        <v>120.3359909057617</v>
       </c>
       <c r="D10" s="2">
-        <v>52.63158084949237</v>
+        <v>52.63157943392434</v>
       </c>
       <c r="E10" s="2">
-        <v>10461.07468122497</v>
+        <v>10461.07691770694</v>
       </c>
       <c r="F10" s="3">
-        <v>0.5780690312385559</v>
+        <v>0.5780689716339111</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1054,19 +1054,19 @@
         <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C11" s="3">
-        <v>120.9140472412109</v>
+        <v>120.9140625</v>
       </c>
       <c r="D11" s="2">
-        <v>52.63158220081687</v>
+        <v>52.63158153042787</v>
       </c>
       <c r="E11" s="2">
-        <v>10487.09541267698</v>
+        <v>10487.09765128837</v>
       </c>
       <c r="F11" s="3">
-        <v>0.5793974995613098</v>
+        <v>0.579397439956665</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1074,16 +1074,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C12" s="3">
-        <v>121.4934463500977</v>
+        <v>121.4934616088867</v>
       </c>
       <c r="D12" s="2">
-        <v>52.631583105755</v>
+        <v>52.63158315858891</v>
       </c>
       <c r="E12" s="2">
-        <v>10537.09555155619</v>
+        <v>10537.09779531127</v>
       </c>
     </row>
   </sheetData>
@@ -1131,7 +1131,7 @@
         <v>10</v>
       </c>
       <c r="B2" s="2">
-        <v>85.90139770507812</v>
+        <v>85.90139007568359</v>
       </c>
       <c r="C2" s="3">
         <v>0</v>
@@ -1171,7 +1171,7 @@
         <v>12</v>
       </c>
       <c r="B4" s="2">
-        <v>86.25180816650391</v>
+        <v>86.25180053710938</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -1191,7 +1191,7 @@
         <v>13</v>
       </c>
       <c r="B5" s="2">
-        <v>88.83446502685547</v>
+        <v>88.83444976806641</v>
       </c>
       <c r="C5" s="3">
         <v>0</v>
@@ -1211,7 +1211,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2">
-        <v>89.82654571533203</v>
+        <v>89.82655334472656</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
@@ -1231,16 +1231,16 @@
         <v>15</v>
       </c>
       <c r="B7" s="2">
-        <v>87.81401824951172</v>
+        <v>87.81401062011719</v>
       </c>
       <c r="C7" s="3">
         <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>9351.73454284668</v>
+        <v>9351.734466552734</v>
       </c>
       <c r="E7" s="2">
-        <v>10229.8747253418</v>
+        <v>10229.87457275391</v>
       </c>
       <c r="F7" s="3">
         <v>10</v>
@@ -1251,7 +1251,7 @@
         <v>16</v>
       </c>
       <c r="B8" s="2">
-        <v>86.81147766113281</v>
+        <v>86.81148529052734</v>
       </c>
       <c r="C8" s="3">
         <v>20</v>
@@ -1260,7 +1260,7 @@
         <v>8523.594360351562</v>
       </c>
       <c r="E8" s="2">
-        <v>10259.82391357422</v>
+        <v>10259.82406616211</v>
       </c>
       <c r="F8" s="3">
         <v>10</v>
@@ -1271,16 +1271,16 @@
         <v>17</v>
       </c>
       <c r="B9" s="2">
-        <v>87.20166015625</v>
+        <v>87.20166778564453</v>
       </c>
       <c r="C9" s="3">
         <v>30</v>
       </c>
       <c r="D9" s="2">
-        <v>7705.479583740234</v>
+        <v>7705.479507446289</v>
       </c>
       <c r="E9" s="2">
-        <v>10321.52938842773</v>
+        <v>10321.52954101562</v>
       </c>
       <c r="F9" s="3">
         <v>10</v>
@@ -1291,16 +1291,16 @@
         <v>18</v>
       </c>
       <c r="B10" s="2">
-        <v>86.49485778808594</v>
+        <v>86.49486541748047</v>
       </c>
       <c r="C10" s="3">
         <v>40</v>
       </c>
       <c r="D10" s="2">
-        <v>6883.462982177734</v>
+        <v>6883.462829589844</v>
       </c>
       <c r="E10" s="2">
-        <v>10343.25729370117</v>
+        <v>10343.25744628906</v>
       </c>
       <c r="F10" s="3">
         <v>10</v>
@@ -1311,16 +1311,16 @@
         <v>19</v>
       </c>
       <c r="B11" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C11" s="3">
         <v>50</v>
       </c>
       <c r="D11" s="2">
-        <v>6068.514404296875</v>
+        <v>6068.514175415039</v>
       </c>
       <c r="E11" s="2">
-        <v>10383.34136962891</v>
+        <v>10383.3415222168</v>
       </c>
       <c r="F11" s="3">
         <v>-5</v>
@@ -1331,16 +1331,16 @@
         <v>19</v>
       </c>
       <c r="B12" s="2">
-        <v>86.29653930664062</v>
+        <v>86.29654693603516</v>
       </c>
       <c r="C12" s="3">
         <v>45</v>
       </c>
       <c r="D12" s="2">
-        <v>6549.997100830078</v>
+        <v>6549.996910095215</v>
       </c>
       <c r="E12" s="2">
-        <v>10433.34136962891</v>
+        <v>10433.3415222168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>